<commit_message>
starting to read from excel
</commit_message>
<xml_diff>
--- a/bin/Debug/Inventory_Stock_Keeping_Application.xlsx
+++ b/bin/Debug/Inventory_Stock_Keeping_Application.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brkkr\source\repos\Inventory-Stock-Keeping-Application\Inventory-Stock-Keeping-Application\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753B9A33-E657-4656-AA90-A64518AC8F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754E5141-4403-43CE-9180-5D40AF7D2DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F43C55A-B955-4DBA-9599-AC3D667DCFFB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>3kohm</t>
+  </si>
+  <si>
+    <t>2kohm</t>
+  </si>
+  <si>
+    <t>1.5kohm</t>
   </si>
 </sst>
 </file>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D9D2ED-B955-4E58-BB5D-50518701EB91}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,6 +495,57 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>12346</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>220</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>12347</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>315</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>